<commit_message>
09.01.2020 Mugdho Corporation Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Cash A.xlsx
+++ b/2020/Others/Cash A.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B597321A-42C8-4299-B4B3-292AF7613A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1700E4CE-BD9D-4608-8C9A-730CA856CE28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,7 +134,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -509,12 +509,42 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -524,32 +554,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -566,52 +588,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -619,43 +628,34 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2581,60 +2581,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -2643,10 +2643,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="47"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2661,10 +2661,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="42"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2680,10 +2680,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="42"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2699,10 +2699,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="42"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2718,10 +2718,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="42"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2737,8 +2737,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2754,8 +2754,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2768,10 +2768,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="47"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2818,58 +2818,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="48"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="48" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -2879,11 +2879,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
@@ -2958,60 +2958,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
     </row>
     <row r="29" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
@@ -3020,10 +3020,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="E31" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="47"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -3038,10 +3038,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="42">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="42"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -3057,10 +3057,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="42">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="42"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -3076,10 +3076,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="42">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="42"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -3095,10 +3095,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="42">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="42"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -3114,8 +3114,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -3131,8 +3131,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3145,10 +3145,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="49"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -3195,58 +3195,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="40"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="40" t="s">
+      <c r="H42" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
@@ -3256,11 +3256,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
@@ -3288,6 +3288,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -3300,32 +3326,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -3338,7 +3338,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3357,66 +3357,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
       <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="85">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="66">
         <f ca="1">TODAY()</f>
-        <v>43832</v>
-      </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
+        <v>43839</v>
+      </c>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
       <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3426,10 +3426,10 @@
       <c r="D5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="61"/>
       <c r="G5" s="27" t="s">
         <v>5</v>
       </c>
@@ -3444,13 +3444,13 @@
       <c r="D6" s="28">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>0</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="62">
+        <v>92</v>
+      </c>
+      <c r="F6" s="62"/>
       <c r="G6" s="28">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>0</v>
+        <v>92000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -3463,13 +3463,13 @@
       <c r="D7" s="28">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>0</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="62">
+        <v>368</v>
+      </c>
+      <c r="F7" s="62"/>
       <c r="G7" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>184000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -3482,13 +3482,13 @@
       <c r="D8" s="28">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>0</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="62">
+        <v>240</v>
+      </c>
+      <c r="F8" s="62"/>
       <c r="G8" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3501,10 +3501,8 @@
       <c r="D9" s="28">
         <v>50</v>
       </c>
-      <c r="E9" s="54">
-        <v>0</v>
-      </c>
-      <c r="F9" s="54"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
       <c r="G9" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3520,10 +3518,8 @@
       <c r="D10" s="28">
         <v>20</v>
       </c>
-      <c r="E10" s="54">
-        <v>0</v>
-      </c>
-      <c r="F10" s="54"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3539,10 +3535,8 @@
       <c r="D11" s="28">
         <v>10</v>
       </c>
-      <c r="E11" s="54">
-        <v>0</v>
-      </c>
-      <c r="F11" s="54"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
       <c r="G11" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3555,14 +3549,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="54"/>
+      <c r="E12" s="62"/>
       <c r="F12" s="28"/>
       <c r="G12" s="22">
         <f>SUM(G6:G11)</f>
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3654,11 +3648,11 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="56" t="s">
+      <c r="H19" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
@@ -3668,9 +3662,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
@@ -3757,66 +3751,66 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
     </row>
     <row r="29" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
     </row>
     <row r="30" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
       <c r="K30" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="84" t="s">
+      <c r="A31" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="84"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="84"/>
-      <c r="E31" s="85">
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="66">
         <f ca="1">E4</f>
-        <v>43832</v>
-      </c>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="83"/>
-      <c r="J31" s="83"/>
+        <v>43839</v>
+      </c>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
     </row>
     <row r="32" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
@@ -3825,10 +3819,10 @@
       <c r="D32" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="61"/>
       <c r="G32" s="27" t="s">
         <v>5</v>
       </c>
@@ -3843,14 +3837,14 @@
       <c r="D33" s="32">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <f>E6</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="62">
+        <f t="shared" ref="E33:E38" si="1">E6</f>
+        <v>92</v>
+      </c>
+      <c r="F33" s="62"/>
       <c r="G33" s="32">
-        <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>0</v>
+        <f t="shared" ref="G33:G38" si="2">SUM(D33*E33)</f>
+        <v>92000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3863,14 +3857,14 @@
       <c r="D34" s="32">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <f>E7</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="62">
+        <f t="shared" si="1"/>
+        <v>368</v>
+      </c>
+      <c r="F34" s="62"/>
       <c r="G34" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>184000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3883,14 +3877,14 @@
       <c r="D35" s="32">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <f>E8</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="62">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="F35" s="62"/>
       <c r="G35" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>24000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3903,13 +3897,10 @@
       <c r="D36" s="32">
         <v>50</v>
       </c>
-      <c r="E36" s="54">
-        <f>E9</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="54"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
       <c r="G36" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H36" s="26"/>
@@ -3923,11 +3914,8 @@
       <c r="D37" s="32">
         <v>20</v>
       </c>
-      <c r="E37" s="54">
-        <f>E10</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="54"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="32">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3943,13 +3931,10 @@
       <c r="D38" s="32">
         <v>10</v>
       </c>
-      <c r="E38" s="54">
-        <f>E11</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="54"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
       <c r="G38" s="32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H38" s="26"/>
@@ -3967,7 +3952,7 @@
       <c r="F39" s="32"/>
       <c r="G39" s="23">
         <f>SUM(G33:G38)</f>
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -4029,25 +4014,25 @@
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="61"/>
+      <c r="D44" s="56"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="61"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="61"/>
+      <c r="D45" s="56"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="61"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="34"/>
@@ -4060,12 +4045,12 @@
       <c r="E46" s="35"/>
       <c r="F46" s="35"/>
       <c r="G46" s="35"/>
-      <c r="H46" s="62" t="str">
+      <c r="H46" s="57" t="str">
         <f>H19</f>
         <v>Jafor Iqbal</v>
       </c>
-      <c r="I46" s="62"/>
-      <c r="J46" s="62"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
@@ -4075,12 +4060,33 @@
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -4096,27 +4102,6 @@
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="A31:D31"/>
     <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -4147,63 +4132,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4213,10 +4198,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="47"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4231,10 +4216,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="42"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -4250,10 +4235,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="42"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -4269,10 +4254,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="42"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -4288,10 +4273,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="42"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4307,10 +4292,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="42"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4326,8 +4311,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4340,10 +4325,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="47"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4390,76 +4375,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="48"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="48" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="66"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
@@ -4534,60 +4519,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
     </row>
     <row r="29" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
@@ -4596,10 +4581,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="65" t="s">
+      <c r="E31" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="71"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4614,10 +4599,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="68">
+      <c r="E32" s="70">
         <v>68</v>
       </c>
-      <c r="F32" s="68"/>
+      <c r="F32" s="70"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4633,10 +4618,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="68">
+      <c r="E33" s="70">
         <v>135</v>
       </c>
-      <c r="F33" s="68"/>
+      <c r="F33" s="70"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4652,10 +4637,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="68">
+      <c r="E34" s="70">
         <v>53</v>
       </c>
-      <c r="F34" s="68"/>
+      <c r="F34" s="70"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4671,10 +4656,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="68">
+      <c r="E35" s="70">
         <v>2</v>
       </c>
-      <c r="F35" s="68"/>
+      <c r="F35" s="70"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4690,10 +4675,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="68">
+      <c r="E36" s="70">
         <v>5</v>
       </c>
-      <c r="F36" s="68"/>
+      <c r="F36" s="70"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4709,8 +4694,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4723,10 +4708,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="69"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4773,76 +4758,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="40"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="40" t="s">
+      <c r="H42" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="41"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="56" t="s">
+      <c r="A46" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="56"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
@@ -4870,6 +4855,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4886,30 +4895,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4941,63 +4926,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5007,10 +4992,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="47"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -5025,10 +5010,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="42"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -5044,10 +5029,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="42"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -5063,10 +5048,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="42"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -5082,8 +5067,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5099,8 +5084,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5116,8 +5101,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5130,10 +5115,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="47"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -5180,72 +5165,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="48"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="48" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="69"/>
-      <c r="B20" s="69"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
@@ -5320,60 +5305,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
     </row>
     <row r="29" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
@@ -5382,10 +5367,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="E31" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="47"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -5400,10 +5385,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="42">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="42"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -5419,10 +5404,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="42">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="42"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -5438,10 +5423,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="42">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="42"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -5457,8 +5442,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5474,8 +5459,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5491,8 +5476,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5505,10 +5490,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="70" t="s">
+      <c r="D38" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="70"/>
+      <c r="E38" s="72"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5555,72 +5540,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="40"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="40" t="s">
+      <c r="H42" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="43"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="56"/>
-      <c r="B46" s="56"/>
+      <c r="A46" s="67"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
@@ -5648,16 +5633,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5670,24 +5663,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5712,64 +5697,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5780,8 +5765,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5792,8 +5777,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5804,8 +5789,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5816,8 +5801,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5828,8 +5813,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5840,8 +5825,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5851,8 +5836,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5896,52 +5881,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="48"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -5951,9 +5936,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
@@ -6040,60 +6025,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -6104,10 +6089,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="65" t="s">
+      <c r="E32" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="71"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -6122,10 +6107,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="42">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="42"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -6141,10 +6126,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="42">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="42"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -6160,10 +6145,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="42">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="42"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -6179,8 +6164,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6196,8 +6181,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -6213,10 +6198,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="68">
+      <c r="E38" s="70">
         <v>100</v>
       </c>
-      <c r="F38" s="68"/>
+      <c r="F38" s="70"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -6229,10 +6214,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="71" t="s">
+      <c r="D39" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="72"/>
+      <c r="E39" s="75"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -6279,58 +6264,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="40"/>
+      <c r="B43" s="50"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="40" t="s">
+      <c r="H43" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="43"/>
+      <c r="B45" s="43"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="40"/>
-      <c r="J46" s="40"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
@@ -6340,12 +6325,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -6358,32 +6369,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6409,177 +6394,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="82">
+      <c r="A5" s="84">
         <v>1</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="73">
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="83">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="82"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="73"/>
+      <c r="A6" s="84"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="83"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="82">
+      <c r="A7" s="84">
         <v>2</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="73">
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="83">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="82"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="73"/>
+      <c r="A8" s="84"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="83"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="82">
+      <c r="A9" s="84">
         <v>3</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="73">
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="83">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="82"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="73"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="83"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="82">
+      <c r="A11" s="84">
         <v>4</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="73">
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="83">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="82"/>
-      <c r="B12" s="79"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="73"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="83"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="73">
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="83">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="73"/>
+      <c r="A14" s="85"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="83"/>
     </row>
     <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
     </row>
     <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -6590,10 +6575,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="65" t="s">
+      <c r="E25" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="65"/>
+      <c r="F25" s="71"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6608,8 +6593,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6625,10 +6610,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="42"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6644,8 +6629,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6661,10 +6646,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="42">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="42"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6680,8 +6665,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6697,10 +6682,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="68">
+      <c r="E31" s="70">
         <v>2</v>
       </c>
-      <c r="F31" s="68"/>
+      <c r="F31" s="70"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6713,10 +6698,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="71" t="s">
+      <c r="D32" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="72"/>
+      <c r="E32" s="75"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6763,58 +6748,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="40"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="40" t="s">
+      <c r="H36" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
     </row>
     <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="41" t="s">
+      <c r="H39" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="40"/>
-      <c r="J39" s="40"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
@@ -6824,12 +6809,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6846,23 +6848,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
02.03.2020 MC Sales Detils
</commit_message>
<xml_diff>
--- a/2020/Others/Cash A.xlsx
+++ b/2020/Others/Cash A.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="31">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -122,10 +122,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Jafor Iqbal</t>
-  </si>
-  <si>
-    <t>Date:</t>
+    <t>Rahinul Kabir</t>
   </si>
 </sst>
 </file>
@@ -133,9 +130,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="[$-809]d\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +284,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -417,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -493,9 +497,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,8 +509,32 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -517,6 +542,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -526,32 +554,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -559,67 +579,42 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -627,33 +622,36 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -693,7 +691,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -743,7 +741,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -793,7 +791,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -843,7 +841,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -898,7 +896,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -948,7 +946,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -998,7 +996,7 @@
         <xdr:cNvPr id="16" name="Straight Connector 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1048,7 +1046,7 @@
         <xdr:cNvPr id="17" name="Straight Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1098,7 +1096,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F693EA6-49EB-42D1-B3CA-F15B26A03B41}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1148,7 +1146,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{92F56342-A68C-4CDA-AD91-6E5E5C5CBD6D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92F56342-A68C-4CDA-AD91-6E5E5C5CBD6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1198,7 +1196,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{334CB43E-1331-4297-A64C-0895C28A3BBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1248,7 +1246,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0D774EF-0DA8-4AF5-A477-477DFA29C2B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1298,7 +1296,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2A810E-B364-491B-AB34-AE585B8D27E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1310,7 +1308,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1348,7 +1346,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBEAD3A6-FB1B-45D2-BDBE-713A9FCBE3DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1360,7 +1358,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1403,7 +1401,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1453,7 +1451,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1503,7 +1501,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1553,7 +1551,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1603,7 +1601,7 @@
         <xdr:cNvPr id="6" name="Straight Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1658,7 +1656,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1708,7 +1706,7 @@
         <xdr:cNvPr id="8" name="Straight Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1758,7 +1756,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1808,7 +1806,7 @@
         <xdr:cNvPr id="10" name="Straight Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1858,7 +1856,7 @@
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1908,7 +1906,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1958,7 +1956,7 @@
         <xdr:cNvPr id="13" name="Straight Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2013,7 +2011,7 @@
         <xdr:cNvPr id="2" name="Straight Connector 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2063,7 +2061,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2113,7 +2111,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2163,7 +2161,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2218,7 +2216,7 @@
         <xdr:cNvPr id="4" name="Straight Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2268,7 +2266,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2558,7 +2556,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2580,60 +2578,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2642,10 +2640,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2660,10 +2658,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="40">
         <v>50</v>
       </c>
-      <c r="F6" s="43"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2679,10 +2677,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="40">
         <v>16</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2698,10 +2696,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="40">
         <v>151</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2717,10 +2715,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="40">
         <v>58</v>
       </c>
-      <c r="F9" s="43"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2736,8 +2734,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2753,8 +2751,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2767,10 +2765,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2817,44 +2815,44 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="42"/>
@@ -2864,11 +2862,11 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2878,11 +2876,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2957,32 +2955,32 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
       <c r="A29" s="46" t="s">
@@ -2999,18 +2997,18 @@
       <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -3019,10 +3017,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="48"/>
+      <c r="F31" s="36"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -3037,10 +3035,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="40">
         <v>50</v>
       </c>
-      <c r="F32" s="43"/>
+      <c r="F32" s="40"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -3056,10 +3054,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="40">
         <v>116</v>
       </c>
-      <c r="F33" s="43"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -3075,10 +3073,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="40">
         <v>151</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="40"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -3094,10 +3092,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="40">
         <v>58</v>
       </c>
-      <c r="F35" s="43"/>
+      <c r="F35" s="40"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -3113,8 +3111,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -3130,8 +3128,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3144,10 +3142,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="40"/>
+      <c r="E38" s="48"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -3194,20 +3192,20 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="49"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="42"/>
@@ -3244,8 +3242,8 @@
       <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="49"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -3255,11 +3253,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3287,6 +3285,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -3299,32 +3323,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -3336,8 +3334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3356,66 +3354,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
       <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
       <c r="K3" s="24"/>
     </row>
-    <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="57">
+    <row r="4" spans="1:11" ht="26.25">
+      <c r="A4" s="83">
         <f ca="1">TODAY()</f>
-        <v>43887</v>
-      </c>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
+        <v>43892</v>
+      </c>
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
       <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3425,10 +3421,10 @@
       <c r="D5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="27" t="s">
         <v>5</v>
       </c>
@@ -3443,13 +3439,13 @@
       <c r="D6" s="28">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>100</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="61">
+        <v>240</v>
+      </c>
+      <c r="F6" s="61"/>
       <c r="G6" s="28">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>100000</v>
+        <v>240000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -3462,13 +3458,13 @@
       <c r="D7" s="28">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>500</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="61">
+        <v>400</v>
+      </c>
+      <c r="F7" s="61"/>
       <c r="G7" s="28">
         <f t="shared" si="0"/>
-        <v>250000</v>
+        <v>200000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -3481,10 +3477,10 @@
       <c r="D8" s="28">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="61">
         <v>100</v>
       </c>
-      <c r="F8" s="54"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="28">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -3500,8 +3496,8 @@
       <c r="D9" s="28">
         <v>50</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
       <c r="G9" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3517,8 +3513,8 @@
       <c r="D10" s="28">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
       <c r="G10" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3534,8 +3530,8 @@
       <c r="D11" s="28">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
       <c r="G11" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3548,14 +3544,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="54"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="28"/>
       <c r="G12" s="22">
         <f>SUM(G6:G11)</f>
-        <v>360000</v>
+        <v>450000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3607,51 +3603,52 @@
       <c r="E16" s="29"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="55" t="s">
+      <c r="H16" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="55"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="29"/>
       <c r="B18" s="29"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="55"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:11" ht="17.25" customHeight="1">
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
       <c r="C19" s="30"/>
-      <c r="D19" s="31" t="s">
-        <v>12</v>
+      <c r="D19" s="35" t="s">
+        <v>30</v>
       </c>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
+      <c r="H19" s="64" t="str">
+        <f>H46</f>
+        <v>Abdul Mannan Tipu</v>
+      </c>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="26"/>
@@ -3661,9 +3658,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="26"/>
@@ -3750,66 +3747,64 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="31.5">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
     </row>
     <row r="29" spans="1:11" ht="18">
-      <c r="A29" s="52" t="s">
+      <c r="A29" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
     </row>
     <row r="30" spans="1:11" ht="18.75">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="59"/>
       <c r="K30" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="40.5" customHeight="1">
-      <c r="A31" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="57">
-        <f ca="1">E4</f>
-        <v>43887</v>
-      </c>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
+    <row r="31" spans="1:11" ht="26.25">
+      <c r="A31" s="83">
+        <f ca="1">TODAY()</f>
+        <v>43892</v>
+      </c>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="83"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="83"/>
+      <c r="J31" s="83"/>
     </row>
     <row r="32" spans="1:11" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3818,10 +3813,10 @@
       <c r="D32" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="27" t="s">
         <v>5</v>
       </c>
@@ -3833,16 +3828,17 @@
       <c r="A33" s="26"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
-      <c r="D33" s="32">
+      <c r="D33" s="31">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>100</v>
-      </c>
-      <c r="F33" s="54"/>
-      <c r="G33" s="32">
+      <c r="E33" s="61">
+        <f>E6</f>
+        <v>240</v>
+      </c>
+      <c r="F33" s="61"/>
+      <c r="G33" s="31">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>100000</v>
+        <v>240000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3852,14 +3848,15 @@
       <c r="A34" s="26"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
-      <c r="D34" s="32">
+      <c r="D34" s="31">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
+      <c r="E34" s="61">
+        <f>E7</f>
         <v>400</v>
       </c>
-      <c r="F34" s="54"/>
-      <c r="G34" s="32">
+      <c r="F34" s="61"/>
+      <c r="G34" s="31">
         <f t="shared" si="1"/>
         <v>200000</v>
       </c>
@@ -3871,14 +3868,17 @@
       <c r="A35" s="26"/>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
-      <c r="D35" s="32">
+      <c r="D35" s="31">
         <v>100</v>
       </c>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="32">
+      <c r="E35" s="61">
+        <f>E8</f>
+        <v>100</v>
+      </c>
+      <c r="F35" s="61"/>
+      <c r="G35" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3888,12 +3888,12 @@
       <c r="A36" s="26"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
-      <c r="D36" s="32">
+      <c r="D36" s="31">
         <v>50</v>
       </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="32">
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3905,12 +3905,12 @@
       <c r="A37" s="26"/>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
-      <c r="D37" s="32">
+      <c r="D37" s="31">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="32">
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="31">
         <f>SUM(D37*E37)</f>
         <v>0</v>
       </c>
@@ -3922,12 +3922,12 @@
       <c r="A38" s="26"/>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
-      <c r="D38" s="32">
+      <c r="D38" s="31">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="32">
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3939,14 +3939,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="66" t="s">
+      <c r="D39" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="67"/>
-      <c r="F39" s="32"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="31"/>
       <c r="G39" s="23">
         <f>SUM(G33:G38)</f>
-        <v>300000</v>
+        <v>450000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3998,53 +3998,52 @@
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
       <c r="G43" s="30"/>
-      <c r="H43" s="55" t="s">
+      <c r="H43" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="63"/>
+      <c r="D44" s="55"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="63"/>
-      <c r="I44" s="63"/>
-      <c r="J44" s="63"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="55"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="32"/>
+      <c r="B45" s="32"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="63"/>
+      <c r="D45" s="55"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="63"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="63"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="35"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="34"/>
       <c r="D46" s="25" t="str">
         <f>D19</f>
-        <v>Rahinul Islam (Kabir)</v>
-      </c>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="64" t="str">
-        <f>H19</f>
-        <v>Jafor Iqbal</v>
-      </c>
-      <c r="I46" s="64"/>
-      <c r="J46" s="64"/>
+        <v>Rahinul Kabir</v>
+      </c>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="21"/>
@@ -4054,12 +4053,33 @@
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="34">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="A31:J31"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -4073,29 +4093,6 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -4126,63 +4123,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4192,10 +4189,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4210,10 +4207,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="40">
         <v>68</v>
       </c>
-      <c r="F6" s="43"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -4229,10 +4226,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="40">
         <v>135</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -4248,10 +4245,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="40">
         <v>53</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -4267,10 +4264,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="40">
         <v>2</v>
       </c>
-      <c r="F9" s="43"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4286,10 +4283,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="40">
         <v>5</v>
       </c>
-      <c r="F10" s="43"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -4305,8 +4302,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4319,10 +4316,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4369,44 +4366,44 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
       <c r="A19" s="42" t="s">
@@ -4418,27 +4415,27 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="69"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4513,32 +4510,32 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
       <c r="A29" s="46" t="s">
@@ -4555,18 +4552,18 @@
       <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4593,10 +4590,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="71">
+      <c r="E32" s="67">
         <v>68</v>
       </c>
-      <c r="F32" s="71"/>
+      <c r="F32" s="67"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4612,10 +4609,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="71">
+      <c r="E33" s="67">
         <v>135</v>
       </c>
-      <c r="F33" s="71"/>
+      <c r="F33" s="67"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4631,10 +4628,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="71">
+      <c r="E34" s="67">
         <v>53</v>
       </c>
-      <c r="F34" s="71"/>
+      <c r="F34" s="67"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4650,10 +4647,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="71">
+      <c r="E35" s="67">
         <v>2</v>
       </c>
-      <c r="F35" s="71"/>
+      <c r="F35" s="67"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4669,10 +4666,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="71">
+      <c r="E36" s="67">
         <v>5</v>
       </c>
-      <c r="F36" s="71"/>
+      <c r="F36" s="67"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4688,8 +4685,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="71"/>
-      <c r="F37" s="71"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="67"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4702,10 +4699,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="70" t="s">
+      <c r="D38" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="70"/>
+      <c r="E38" s="66"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4752,20 +4749,20 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="49"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="42"/>
@@ -4804,24 +4801,24 @@
       <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="49"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4849,6 +4846,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4865,30 +4886,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4920,63 +4917,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4986,10 +4983,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -5004,10 +5001,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="40">
         <v>44</v>
       </c>
-      <c r="F6" s="43"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -5023,10 +5020,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="40">
         <v>118</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -5042,10 +5039,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="40">
         <v>510</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -5061,8 +5058,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5078,8 +5075,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5095,8 +5092,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5109,10 +5106,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -5159,44 +5156,44 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
       <c r="A19" s="42"/>
@@ -5206,25 +5203,25 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="72"/>
-      <c r="B20" s="72"/>
+      <c r="A20" s="70"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5299,32 +5296,32 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
       <c r="A29" s="46" t="s">
@@ -5341,18 +5338,18 @@
       <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -5361,10 +5358,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="48"/>
+      <c r="F31" s="36"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -5379,10 +5376,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="40">
         <v>44</v>
       </c>
-      <c r="F32" s="43"/>
+      <c r="F32" s="40"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -5398,10 +5395,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="40">
         <v>118</v>
       </c>
-      <c r="F33" s="43"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -5417,10 +5414,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="40">
         <v>510</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="40"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -5436,8 +5433,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5453,8 +5450,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5470,8 +5467,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5484,10 +5481,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="73" t="s">
+      <c r="D38" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="73"/>
+      <c r="E38" s="69"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5534,20 +5531,20 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="49"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="42"/>
@@ -5584,22 +5581,22 @@
       <c r="H45" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="49"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5627,16 +5624,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5649,24 +5654,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5691,64 +5688,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5759,8 +5756,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5771,8 +5768,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5783,8 +5780,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5795,8 +5792,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5807,8 +5804,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5819,8 +5816,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5830,8 +5827,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5875,40 +5872,40 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="49"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="42"/>
@@ -5918,9 +5915,9 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5930,9 +5927,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -6019,32 +6016,32 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
       <c r="A30" s="46" t="s">
@@ -6061,18 +6058,18 @@
       <c r="J30" s="46"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -6101,10 +6098,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="40">
         <v>30</v>
       </c>
-      <c r="F33" s="43"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -6120,10 +6117,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="40">
         <v>35</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="40"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -6139,10 +6136,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="40">
         <v>425</v>
       </c>
-      <c r="F35" s="43"/>
+      <c r="F35" s="40"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -6158,8 +6155,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6175,8 +6172,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="71"/>
-      <c r="F37" s="71"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="67"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -6192,10 +6189,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="71">
+      <c r="E38" s="67">
         <v>100</v>
       </c>
-      <c r="F38" s="71"/>
+      <c r="F38" s="67"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -6208,10 +6205,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="74" t="s">
+      <c r="D39" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="75"/>
+      <c r="E39" s="72"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -6258,20 +6255,20 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="41"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="41" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="42"/>
@@ -6308,8 +6305,8 @@
       <c r="H46" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="49"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -6319,12 +6316,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="45"/>
+      <c r="J47" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -6337,32 +6360,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6388,151 +6385,151 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="85">
+      <c r="A5" s="81">
         <v>1</v>
       </c>
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="76">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="80">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="85"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="76"/>
+      <c r="A6" s="81"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="80"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="85">
+      <c r="A7" s="81">
         <v>2</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="76">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="80">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="85"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="76"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="80"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="85">
+      <c r="A9" s="81">
         <v>3</v>
       </c>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="76">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="80">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="85"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="76"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="80"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="85">
+      <c r="A11" s="81">
         <v>4</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="76">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="80">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="85"/>
-      <c r="B12" s="82"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="76"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="80"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="76">
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="80">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="77"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="76"/>
+      <c r="A14" s="82"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="80"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
       <c r="A23" s="46" t="s">
@@ -6549,16 +6546,16 @@
       <c r="J23" s="46"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6587,8 +6584,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6604,10 +6601,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="40">
         <v>30</v>
       </c>
-      <c r="F27" s="43"/>
+      <c r="F27" s="40"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6623,8 +6620,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6640,10 +6637,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="40">
         <v>5</v>
       </c>
-      <c r="F29" s="43"/>
+      <c r="F29" s="40"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6659,8 +6656,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6676,10 +6673,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="71">
+      <c r="E31" s="67">
         <v>2</v>
       </c>
-      <c r="F31" s="71"/>
+      <c r="F31" s="67"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6692,10 +6689,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="74" t="s">
+      <c r="D32" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="75"/>
+      <c r="E32" s="72"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6742,20 +6739,20 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="41"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="41" t="s">
+      <c r="H36" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="42"/>
@@ -6792,8 +6789,8 @@
       <c r="H39" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6803,12 +6800,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6825,23 +6839,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>